<commit_message>
On branch master Changes to be committed: 	modified:   tspi/lau1/infoform-20095495.xlsx 	modified:   tspi/lau1/infoform-20105627.xlsx 	modified:   tspi/lau1/infoform-20105914.xlsx 	modified:   tspi/lau1/infoform-20106065.xlsx 	modified:   tspi/lau1/infoform-20106381.xlsx 	new file:   tspi/templates/infoform.xlsx
</commit_message>
<xml_diff>
--- a/tspi/lau1/infoform-20106065.xlsx
+++ b/tspi/lau1/infoform-20106065.xlsx
@@ -61,13 +61,13 @@
     <t>Briefly describe your work on other team projects</t>
   </si>
   <si>
-    <t>Video juegos con allegro y opengl.</t>
+    <t>Proyectos universitarios.</t>
   </si>
   <si>
     <t>Briefly describe any leadership or management positions you have held(at work or in clubs/organizations)</t>
   </si>
   <si>
-    <t>Ninguna</t>
+    <t>Ninguna.</t>
   </si>
   <si>
     <t>State your team preferences, if any</t>
@@ -142,7 +142,7 @@
     <t>2:00</t>
   </si>
   <si>
-    <t>Clases</t>
+    <t>Ocupado</t>
   </si>
   <si>
     <t>2:30</t>
@@ -401,13 +401,13 @@
   </sheetPr>
   <dimension ref="A2:H58"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A28" view="normal" windowProtection="false" workbookViewId="0" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100">
-      <selection activeCell="E56" activeCellId="0" pane="topLeft" sqref="E56"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100">
+      <selection activeCell="A13" activeCellId="0" pane="topLeft" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="26.1725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="26.3019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="2">
@@ -1089,7 +1089,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1114,7 +1114,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>